<commit_message>
get coordi_pairs and id_pairs(nan-Dam,Niclos)
</commit_message>
<xml_diff>
--- a/data/am_tram12_name.xlsx
+++ b/data/am_tram12_name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UTNCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D68CEE0-25AE-43DA-A9FE-74D291FCB3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DC9BD7-FD2A-4EBC-AED4-F848C9B55636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41625" yWindow="1710" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,10 +75,10 @@
     <t>Nieuwezijds Kolk</t>
   </si>
   <si>
-    <t>Centraal Station</t>
-  </si>
-  <si>
     <t>v. Hilligaertstraat</t>
+  </si>
+  <si>
+    <t>Centraal Station_B</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +431,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -491,7 +491,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>